<commit_message>
Included an optional BLE121 on this module to allow for stand-alone long range operation
</commit_message>
<xml_diff>
--- a/bom/ovrBeaconGateway-wifi_pricing.xlsx
+++ b/bom/ovrBeaconGateway-wifi_pricing.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="ovrBeaconGateway-wifi_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="90">
   <si>
     <t>Reference</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>Assembly</t>
+  </si>
+  <si>
+    <t>Case Print/Machining</t>
   </si>
 </sst>
 </file>
@@ -302,8 +305,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.000000"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -350,9 +353,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -360,22 +363,22 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.000000"/>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -388,8 +391,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J25" totalsRowCount="1">
-  <autoFilter ref="A1:J24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J26" totalsRowCount="1">
+  <autoFilter ref="A1:J25"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Reference"/>
     <tableColumn id="2" name="Manufacturer"/>
@@ -400,12 +403,12 @@
     <tableColumn id="7" name="Price (qty 1)" totalsRowLabel="Total:" dataDxfId="5" dataCellStyle="Currency"/>
     <tableColumn id="9" name="Subtotal (qty 1)" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="1" dataCellStyle="Currency">
       <calculatedColumnFormula>F2*G2</calculatedColumnFormula>
-      <totalsRowFormula>SUM(H2:H24)</totalsRowFormula>
+      <totalsRowFormula>SUM(H2:H25)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="8" name="Price (qty 1000)" dataDxfId="3" dataCellStyle="Currency"/>
     <tableColumn id="10" name="Subtotal (qty 1000)" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>F2*I2</calculatedColumnFormula>
-      <totalsRowFormula>SUM(J2:J24)</totalsRowFormula>
+      <totalsRowFormula>SUM(J2:J25)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -678,10 +681,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -753,14 +756,14 @@
         <v>1.4</v>
       </c>
       <c r="H2" s="1">
-        <f t="shared" ref="H2:H21" si="0">F2*G2</f>
+        <f t="shared" ref="H2:H22" si="0">F2*G2</f>
         <v>1.4</v>
       </c>
       <c r="I2" s="3">
         <v>0.77439999999999998</v>
       </c>
       <c r="J2" s="1">
-        <f t="shared" ref="J2:J21" si="1">F2*I2</f>
+        <f t="shared" ref="J2:J22" si="1">F2*I2</f>
         <v>0.77439999999999998</v>
       </c>
     </row>
@@ -1378,59 +1381,67 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="3">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="J21" s="1">
+        <f>F21*I21</f>
+        <v>4.8899999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>78</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>79</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>80</v>
       </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
         <v>81</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>4</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G22" s="1">
         <v>0.59</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H22" s="1">
         <f t="shared" si="0"/>
         <v>2.36</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I22" s="3">
         <v>0.14404</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J22" s="1">
         <f t="shared" si="1"/>
         <v>0.57616000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="1"/>
-    </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>87</v>
-      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="1">
-        <f>F23*I23</f>
-        <v>0</v>
-      </c>
+      <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1440,17 +1451,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G25" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="1">
+        <f>F25*I25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
         <v>86</v>
       </c>
-      <c r="H25" s="2">
-        <f>SUM(H2:H24)</f>
+      <c r="H26" s="2">
+        <f>SUM(H2:H25)</f>
         <v>27.33</v>
       </c>
-      <c r="J25" s="2">
-        <f>SUM(J2:J24)</f>
-        <v>15.244028</v>
+      <c r="J26" s="2">
+        <f>SUM(J2:J25)</f>
+        <v>20.134028000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM and pricing…still waiting for quote on BLE121
</commit_message>
<xml_diff>
--- a/bom/ovrBeaconGateway-wifi_pricing.xlsx
+++ b/bom/ovrBeaconGateway-wifi_pricing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-1900" yWindow="-19120" windowWidth="28800" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="-4520" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ovrBeaconGateway-wifi_BOM" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="97">
   <si>
     <t>Reference</t>
   </si>
@@ -297,6 +297,27 @@
   </si>
   <si>
     <t>Case Print/Machining</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>BlueGiga</t>
+  </si>
+  <si>
+    <t>BLE121LR-A-M256K</t>
+  </si>
+  <si>
+    <t>1446-1039-1-ND</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>GRM188R71C104KA01D</t>
+  </si>
+  <si>
+    <t>490-1532-1-ND</t>
   </si>
 </sst>
 </file>
@@ -330,12 +351,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -351,11 +378,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -369,7 +397,7 @@
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000000"/>
@@ -391,8 +419,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J26" totalsRowCount="1">
-  <autoFilter ref="A1:J25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J29" totalsRowCount="1">
+  <autoFilter ref="A1:J28"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Reference"/>
     <tableColumn id="2" name="Manufacturer"/>
@@ -403,12 +431,12 @@
     <tableColumn id="7" name="Price (qty 1)" totalsRowLabel="Total:" dataDxfId="5" dataCellStyle="Currency"/>
     <tableColumn id="9" name="Subtotal (qty 1)" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="1" dataCellStyle="Currency">
       <calculatedColumnFormula>F2*G2</calculatedColumnFormula>
-      <totalsRowFormula>SUM(H2:H25)</totalsRowFormula>
+      <totalsRowFormula>SUM(H2:H28)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="8" name="Price (qty 1000)" dataDxfId="3" dataCellStyle="Currency"/>
     <tableColumn id="10" name="Subtotal (qty 1000)" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>F2*I2</calculatedColumnFormula>
-      <totalsRowFormula>SUM(J2:J25)</totalsRowFormula>
+      <totalsRowFormula>SUM(J2:J28)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -681,10 +709,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,14 +784,14 @@
         <v>1.4</v>
       </c>
       <c r="H2" s="1">
-        <f t="shared" ref="H2:H22" si="0">F2*G2</f>
+        <f t="shared" ref="H2:H24" si="0">F2*G2</f>
         <v>1.4</v>
       </c>
       <c r="I2" s="3">
         <v>0.77439999999999998</v>
       </c>
-      <c r="J2" s="1">
-        <f t="shared" ref="J2:J22" si="1">F2*I2</f>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J24" si="1">F2*I2</f>
         <v>0.77439999999999998</v>
       </c>
     </row>
@@ -796,7 +824,7 @@
       <c r="I3" s="3">
         <v>0.35102</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="3">
         <f t="shared" si="1"/>
         <v>0.35102</v>
       </c>
@@ -830,7 +858,7 @@
       <c r="I4" s="3">
         <v>0.48620000000000002</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="3">
         <f t="shared" si="1"/>
         <v>0.48620000000000002</v>
       </c>
@@ -864,7 +892,7 @@
       <c r="I5" s="3">
         <v>0.93930000000000002</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="3">
         <f t="shared" si="1"/>
         <v>0.93930000000000002</v>
       </c>
@@ -898,7 +926,7 @@
       <c r="I6" s="3">
         <v>1.68</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="3">
         <f t="shared" si="1"/>
         <v>1.68</v>
       </c>
@@ -932,7 +960,7 @@
       <c r="I7" s="3">
         <v>2.85</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="3">
         <f t="shared" si="1"/>
         <v>2.85</v>
       </c>
@@ -966,7 +994,7 @@
       <c r="I8" s="3">
         <v>5.5399999999999998E-3</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="3">
         <f t="shared" si="1"/>
         <v>1.6619999999999999E-2</v>
       </c>
@@ -1000,7 +1028,7 @@
       <c r="I9" s="3">
         <v>5.0500000000000003E-2</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="3">
         <f t="shared" si="1"/>
         <v>0.15150000000000002</v>
       </c>
@@ -1034,7 +1062,7 @@
       <c r="I10" s="3">
         <v>7.5649999999999995E-2</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="3">
         <f t="shared" si="1"/>
         <v>7.5649999999999995E-2</v>
       </c>
@@ -1068,7 +1096,7 @@
       <c r="I11" s="3">
         <v>7.5649999999999995E-2</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="3">
         <f t="shared" si="1"/>
         <v>7.5649999999999995E-2</v>
       </c>
@@ -1102,7 +1130,7 @@
       <c r="I12" s="3">
         <v>3.6099999999999999E-3</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="3">
         <f t="shared" si="1"/>
         <v>2.1659999999999999E-2</v>
       </c>
@@ -1136,7 +1164,7 @@
       <c r="I13" s="3">
         <v>5.5399999999999998E-3</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="3">
         <f t="shared" si="1"/>
         <v>5.5399999999999998E-3</v>
       </c>
@@ -1170,7 +1198,7 @@
       <c r="I14" s="3">
         <v>3.6099999999999999E-3</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="3">
         <f t="shared" si="1"/>
         <v>2.1659999999999999E-2</v>
       </c>
@@ -1204,7 +1232,7 @@
       <c r="I15" s="3">
         <v>0.27555000000000002</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="3">
         <f t="shared" si="1"/>
         <v>0.27555000000000002</v>
       </c>
@@ -1238,7 +1266,7 @@
       <c r="I16" s="3">
         <v>3.954E-3</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="3">
         <f t="shared" si="1"/>
         <v>7.9080000000000001E-3</v>
       </c>
@@ -1272,7 +1300,7 @@
       <c r="I17" s="3">
         <v>3.95</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="3">
         <f t="shared" si="1"/>
         <v>3.95</v>
       </c>
@@ -1306,7 +1334,7 @@
       <c r="I18" s="3">
         <v>8.5769999999999999E-2</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="3">
         <f t="shared" si="1"/>
         <v>8.5769999999999999E-2</v>
       </c>
@@ -1340,63 +1368,75 @@
       <c r="I19" s="3">
         <v>0.64944000000000002</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="3">
         <f t="shared" si="1"/>
         <v>0.64944000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" s="1">
-        <v>3.36</v>
+        <v>13.76</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="0"/>
-        <v>3.36</v>
-      </c>
-      <c r="I20" s="3">
-        <v>2.25</v>
-      </c>
-      <c r="J20" s="1">
-        <f t="shared" si="1"/>
-        <v>2.25</v>
+        <f>F20*G20</f>
+        <v>13.76</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4">
+        <f>F20*I20</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>96</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="G21" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H21" s="1">
+        <f>F21*G21</f>
+        <v>0.1</v>
+      </c>
       <c r="I21" s="3">
-        <v>4.8899999999999997</v>
-      </c>
-      <c r="J21" s="1">
+        <v>4.7299999999999998E-3</v>
+      </c>
+      <c r="J21" s="3">
         <f>F21*I21</f>
-        <v>4.8899999999999997</v>
+        <v>4.7299999999999998E-3</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1422,58 +1462,134 @@
         <v>0.59</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="0"/>
+        <f>F22*G22</f>
         <v>2.36</v>
       </c>
       <c r="I22" s="3">
         <v>0.14404</v>
       </c>
-      <c r="J22" s="1">
-        <f t="shared" si="1"/>
+      <c r="J22" s="3">
+        <f>F22*I22</f>
         <v>0.57616000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1">
+        <f>F23*G23</f>
+        <v>0</v>
+      </c>
       <c r="I23" s="3"/>
-      <c r="J23" s="1"/>
+      <c r="J23" s="3">
+        <f>F23*I23</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>87</v>
-      </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="1">
-        <f>F24*I24</f>
-        <v>0</v>
+        <v>75</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>3.36</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="0"/>
+        <v>3.36</v>
+      </c>
+      <c r="I24" s="3">
+        <v>2.25</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="1">
+      <c r="I25" s="3">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="J25" s="3">
         <f>F25*I25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G26" t="s">
+        <v>4.8899999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3">
+        <f>F27*I27</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="3">
+        <v>2</v>
+      </c>
+      <c r="J28" s="3">
+        <f>F28*I28</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
         <v>86</v>
       </c>
-      <c r="H26" s="2">
-        <f>SUM(H2:H25)</f>
-        <v>27.33</v>
-      </c>
-      <c r="J26" s="2">
-        <f>SUM(J2:J25)</f>
-        <v>20.134028000000001</v>
+      <c r="H29" s="2">
+        <f>SUM(H2:H28)</f>
+        <v>41.19</v>
+      </c>
+      <c r="J29" s="2">
+        <f>SUM(J2:J28)</f>
+        <v>23.138757999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added price for BLE121
</commit_message>
<xml_diff>
--- a/bom/ovrBeaconGateway-wifi_pricing.xlsx
+++ b/bom/ovrBeaconGateway-wifi_pricing.xlsx
@@ -351,18 +351,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -383,7 +377,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -394,13 +388,13 @@
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000000"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
@@ -429,12 +423,12 @@
     <tableColumn id="5" name="Supplier Part Num."/>
     <tableColumn id="6" name="Quantity"/>
     <tableColumn id="7" name="Price (qty 1)" totalsRowLabel="Total:" dataDxfId="5" dataCellStyle="Currency"/>
-    <tableColumn id="9" name="Subtotal (qty 1)" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="1" dataCellStyle="Currency">
+    <tableColumn id="9" name="Subtotal (qty 1)" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="3" dataCellStyle="Currency">
       <calculatedColumnFormula>F2*G2</calculatedColumnFormula>
       <totalsRowFormula>SUM(H2:H28)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="Price (qty 1000)" dataDxfId="3" dataCellStyle="Currency"/>
-    <tableColumn id="10" name="Subtotal (qty 1000)" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="8" name="Price (qty 1000)" dataDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="10" name="Subtotal (qty 1000)" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>F2*I2</calculatedColumnFormula>
       <totalsRowFormula>SUM(J2:J28)</totalsRowFormula>
     </tableColumn>
@@ -712,7 +706,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1399,10 +1393,12 @@
         <f>F20*G20</f>
         <v>13.76</v>
       </c>
-      <c r="I20" s="4"/>
+      <c r="I20" s="4">
+        <v>8.3123199999999997</v>
+      </c>
       <c r="J20" s="4">
         <f>F20*I20</f>
-        <v>0</v>
+        <v>8.3123199999999997</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1475,15 +1471,9 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G23" s="1"/>
-      <c r="H23" s="1">
-        <f>F23*G23</f>
-        <v>0</v>
-      </c>
+      <c r="H23" s="1"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="3">
-        <f>F23*I23</f>
-        <v>0</v>
-      </c>
+      <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -1589,7 +1579,7 @@
       </c>
       <c r="J29" s="2">
         <f>SUM(J2:J28)</f>
-        <v>23.138757999999999</v>
+        <v>31.451077999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>